<commit_message>
Updated Excel and added Info Package
</commit_message>
<xml_diff>
--- a/BroadclothSolution/BISolutionWorksheets.xlsx
+++ b/BroadclothSolution/BISolutionWorksheets.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f0a969d3d8ed1004/DU/Fall 2017/INFO 3300/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zach Burmeister\OneDrive\DU\Fall 2017\INFO 3300\Broadcloth Solution\BroadclothSolution\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="A80B3C196C0FF85611C780D46C7EE440B91C2B05" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21" xr10:uidLastSave="{507B2316-F25A-405D-8B7A-EA6A28AB84FA}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="23" windowWidth="22980" windowHeight="12165" tabRatio="950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="23" windowWidth="22980" windowHeight="12165" tabRatio="950" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team Members" sheetId="7" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="227">
   <si>
     <t>Object Name</t>
   </si>
@@ -34,9 +35,6 @@
     <t>Source</t>
   </si>
   <si>
-    <t>Pubs.dbo.Sales</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -49,15 +47,9 @@
     <t>Data Warehouse</t>
   </si>
   <si>
-    <t>Pubs OLTP</t>
-  </si>
-  <si>
     <t>Measure Column</t>
   </si>
   <si>
-    <t>Pubs.dbo.Sales.Qty</t>
-  </si>
-  <si>
     <t>Table</t>
   </si>
   <si>
@@ -67,9 +59,6 @@
     <t>Destination Type</t>
   </si>
   <si>
-    <t>Pubs.dbo.Sales.Title_id</t>
-  </si>
-  <si>
     <t>int</t>
   </si>
   <si>
@@ -322,132 +311,12 @@
     <t>Tim Thomas</t>
   </si>
   <si>
-    <t>DWPubsSales</t>
-  </si>
-  <si>
-    <t>DWPubsSales.dbo.FactSales</t>
-  </si>
-  <si>
-    <t>DWPubsSales.dbo.FactSales.TitleKey</t>
-  </si>
-  <si>
-    <t>DWPubsSales.dbo.DimTitles</t>
-  </si>
-  <si>
-    <t>DWPubsSales.dbo.FactSales.SalesQuantity</t>
-  </si>
-  <si>
-    <t>Pubs.dbo.Sales.Stor_id</t>
-  </si>
-  <si>
-    <t>DWPubsSales.dbo.StoreKey</t>
-  </si>
-  <si>
-    <t>DWPubsSales.dbo.OrderDateKey</t>
-  </si>
-  <si>
-    <t>varchar(6)</t>
-  </si>
-  <si>
-    <t>char(4)</t>
-  </si>
-  <si>
-    <t>varchar(20)</t>
-  </si>
-  <si>
     <t>datetime</t>
   </si>
   <si>
-    <t>Pubs.dbo.stores</t>
-  </si>
-  <si>
-    <t>Pubs.dbo.titles</t>
-  </si>
-  <si>
-    <t>Pubs.dbo.publishers</t>
-  </si>
-  <si>
-    <t>Pubs.dbo.titleauthor</t>
-  </si>
-  <si>
-    <t>Pubs.dbo.authors</t>
-  </si>
-  <si>
-    <t>Pubs.dbo.stores.stor_id</t>
-  </si>
-  <si>
-    <t>Pubs.dbo.stores.stor_name</t>
-  </si>
-  <si>
-    <t>Pubs.dbo.titles.title_id</t>
-  </si>
-  <si>
-    <t>Pubs.dbo.Sales.dbo.ord_num</t>
-  </si>
-  <si>
-    <t>Pubs.dbo.Sales.dbo.ord_date</t>
-  </si>
-  <si>
-    <t>Pubs.dbo.titles.title</t>
-  </si>
-  <si>
-    <t>Pubs.dbo.titles.type</t>
-  </si>
-  <si>
-    <t>Pubs.dbo.titles.pub_id</t>
-  </si>
-  <si>
-    <t>Pubs.dbo.titles.price</t>
-  </si>
-  <si>
-    <t>Pubs.dbo.titles.pubdate</t>
-  </si>
-  <si>
-    <t>Pubs.dbo.publishers.pub_id</t>
-  </si>
-  <si>
-    <t>Pubs.dbo.publishers.pub_name</t>
-  </si>
-  <si>
-    <t>Pubs.dbo.titleauthor.au_ord</t>
-  </si>
-  <si>
-    <t>Pubs.dbo.authors.au_id</t>
-  </si>
-  <si>
-    <t>Pubs.dbo.authors.au_lname</t>
-  </si>
-  <si>
-    <t>Pubs.dbo.authors.state</t>
-  </si>
-  <si>
     <t>Dimesion Table</t>
   </si>
   <si>
-    <t>DWPubsSales.dbo.DimStores</t>
-  </si>
-  <si>
-    <t>DWPubsSales.dbo.DimPublishers</t>
-  </si>
-  <si>
-    <t>DWPubsSales.dbo.DimAuthors</t>
-  </si>
-  <si>
-    <t>Pubs.dbo.authors.au_fname</t>
-  </si>
-  <si>
-    <t>DWPubsSales.dbo.DimAuthors.AuthorName</t>
-  </si>
-  <si>
-    <t>DWPubsSales.dbo.DimAuthors.AuthorState</t>
-  </si>
-  <si>
-    <t>DWPubsSales.dbo.DimAuthors.AuthorId</t>
-  </si>
-  <si>
-    <t>DWPubsSales.dbo.DimAuthors.AuthorKey</t>
-  </si>
-  <si>
     <t>Role</t>
   </si>
   <si>
@@ -466,63 +335,15 @@
     <t>Dimension Column</t>
   </si>
   <si>
-    <t>varchar(11)</t>
-  </si>
-  <si>
-    <t>varchar(40)</t>
-  </si>
-  <si>
-    <t>char(2)</t>
-  </si>
-  <si>
-    <t>varchar(80)</t>
-  </si>
-  <si>
-    <t>char(12)</t>
-  </si>
-  <si>
-    <t>money</t>
-  </si>
-  <si>
-    <t>tinyint</t>
-  </si>
-  <si>
     <t>nvarchar(50)</t>
   </si>
   <si>
-    <t>DWPubsSales.dbo.DimStores.StoresKey</t>
-  </si>
-  <si>
-    <t>DWPubsSales.dbo.DimStores.StoreId</t>
-  </si>
-  <si>
-    <t>DWPubsSales.dbo.DimStores.StoreName</t>
-  </si>
-  <si>
-    <t>Dimension  Column</t>
-  </si>
-  <si>
     <t>Generated</t>
   </si>
   <si>
     <t>na</t>
   </si>
   <si>
-    <t>DWPubsSales.dbo.OrderNumber</t>
-  </si>
-  <si>
-    <t>decimal(18,4)</t>
-  </si>
-  <si>
-    <t>nchar(4)</t>
-  </si>
-  <si>
-    <t>nchar(6)</t>
-  </si>
-  <si>
-    <t>nchar(11)</t>
-  </si>
-  <si>
     <t>Data Warehouse Objects Worksheet</t>
   </si>
   <si>
@@ -571,102 +392,15 @@
     <t>SSIS ETL Objects Worksheet</t>
   </si>
   <si>
-    <t>DWPubsSales.dbo.FactTitlesAuthors</t>
-  </si>
-  <si>
-    <t>DWPubsSales.dbo.FactTitlesAuthorsKey</t>
-  </si>
-  <si>
-    <t>DWPubsSales.dbo.FactTitlesAuthors.TitleKey</t>
-  </si>
-  <si>
-    <t>DWPubsSales.dbo.FactTitlesAuthors.AuthorOrder</t>
-  </si>
-  <si>
     <t>SSAS Objects Worksheet</t>
   </si>
   <si>
-    <t>DWPubsSales.dbo.DimTitles.TitleKey</t>
-  </si>
-  <si>
-    <t>DWPubsSales.dbo.DimTitles.TitleId</t>
-  </si>
-  <si>
-    <t>DWPubsSales.dbo.DimTitles.TitleName</t>
-  </si>
-  <si>
-    <t>DWPubsSales.dbo.DimTitles.TitleType</t>
-  </si>
-  <si>
-    <t>DWPubsSales.dbo.DimTitles.PublisherId</t>
-  </si>
-  <si>
-    <t>DWPubsSales.dbo.DimTitles.TitlePrice</t>
-  </si>
-  <si>
-    <t>DWPubsSales.dbo.DimTitles.PublishedDate</t>
-  </si>
-  <si>
-    <t>DWPubsSales.dbo.DimPublishers.PublisherKey</t>
-  </si>
-  <si>
-    <t>DWPubsSales.dbo.DimPublishers.PublisherId</t>
-  </si>
-  <si>
-    <t>DWPubsSales.dbo.DimPublishers.PublihserName</t>
-  </si>
-  <si>
-    <t>nchar(2)</t>
-  </si>
-  <si>
     <t>Destination</t>
   </si>
   <si>
-    <t>smallint</t>
-  </si>
-  <si>
-    <t>nvarchar(100)</t>
-  </si>
-  <si>
-    <t>Pubs.dbo.titleauthor.au_id</t>
-  </si>
-  <si>
-    <t>Pubs.dbo.titleauthor.title_id</t>
-  </si>
-  <si>
-    <t>DWPubsSales.dbo.DimDates.DateKey</t>
-  </si>
-  <si>
-    <t>DWPubsSales.dbo.DimDates</t>
-  </si>
-  <si>
-    <t>DWPubsSales.dbo.DimDates.DateName</t>
-  </si>
-  <si>
-    <t>DWPubsSales.dbo.DimDates.MonthName</t>
-  </si>
-  <si>
-    <t>DWPubsSales.dbo.DimDates.Quarter</t>
-  </si>
-  <si>
-    <t>DWPubsSales.dbo.DimDates.Month</t>
-  </si>
-  <si>
-    <t>DWPubsSales.dbo.DimDates.QuarterName</t>
-  </si>
-  <si>
-    <t>DWPubsSales.dbo.DimDates.Year</t>
-  </si>
-  <si>
-    <t>DWPubsSales.dbo.DimDates.YearName</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
-    <t>DWPubsSales.dbo.DimDates.Date</t>
-  </si>
-  <si>
     <t>Zach Burmeister</t>
   </si>
   <si>
@@ -677,6 +411,303 @@
   </si>
   <si>
     <t>Julia Tremaroli</t>
+  </si>
+  <si>
+    <t>DWBroadcloth</t>
+  </si>
+  <si>
+    <t>Broadcloth OLTP</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.FactProduction</t>
+  </si>
+  <si>
+    <t>Broadcloth.dbo.ProductionBatch</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.DimProductionBatch.FactoryID</t>
+  </si>
+  <si>
+    <t>Broadcloth.dbo.ProductionBatch.FactoryID</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.DimProductionBatch.ItemID</t>
+  </si>
+  <si>
+    <t>Broadcloth.dbo.ProductionBatch.ItemID</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.DimProductionBatch.StartDateTime</t>
+  </si>
+  <si>
+    <t>Broadcloth.dbo.ProductionBatch.StartDateTime</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.DimProductionBatch.QuantityProduced</t>
+  </si>
+  <si>
+    <t>Broadcloth.dbo.ProductionBatch.QuantityProduced</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.DimProductionBatch.EstEndTime</t>
+  </si>
+  <si>
+    <t>Broadcloth.dbo.ProductionBatch.EstEndTime</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.DimProductionBatch.ActualEndTime</t>
+  </si>
+  <si>
+    <t>Broadcloth.dbo.ProductionBatch.ActualEndTime</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.DimProductionBatch.ProductionCost</t>
+  </si>
+  <si>
+    <t>Broadcloth.dbo.ProductionBatch.ProductionCost</t>
+  </si>
+  <si>
+    <t>numeric(38,4)</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.DimProductionBatch.CostCurrency</t>
+  </si>
+  <si>
+    <t>Broadcloth.dbo.ProductionBatch.CostCurrency</t>
+  </si>
+  <si>
+    <t>nvarchar(5)</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.DimProductionBatch.CostExchangeRate</t>
+  </si>
+  <si>
+    <t>Broadcloth.dbo.ProductionBatch.CostExchangeDate</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.DimProductionBatch.OrderID</t>
+  </si>
+  <si>
+    <t>Broadcloth.dbo.ProductionBatch.OrderID</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.DimProductionBatch.QualityRating</t>
+  </si>
+  <si>
+    <t>Broadcloth.dbo.ProductionBatch.QualityRating</t>
+  </si>
+  <si>
+    <t>numeric(18,0)</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.Shipment</t>
+  </si>
+  <si>
+    <t>Broadcloth.dbo.Shipment</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.DimShipments.ShipmentID</t>
+  </si>
+  <si>
+    <t>Broadcloth.dbo.Shipments.ShipmentID</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.DimShipments.ShipMethod</t>
+  </si>
+  <si>
+    <t>Broadcloth.dbo.Shipments.ShipMethod</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.DimShipments.ShipDate</t>
+  </si>
+  <si>
+    <t>Broadcloth.dbo.Shipments.Shipdate</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.DimShipments.ShipPostal</t>
+  </si>
+  <si>
+    <t>Broadcloth.dbo.Shipments.ShipPostal</t>
+  </si>
+  <si>
+    <t>nvarchar(12)</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.DimShipments.ShipState</t>
+  </si>
+  <si>
+    <t>Broadcloth.dbo.Shipments.ShipState</t>
+  </si>
+  <si>
+    <t>nvarchar(20)</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.DimShipments.ShipNation</t>
+  </si>
+  <si>
+    <t>Broadcloth.dbo.Shipments.ShipNation</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.DimShipments.ShipCurrency</t>
+  </si>
+  <si>
+    <t>Broadcloth.dbo.Shipments.ShipCurrency</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.DimShipmentItem.QuantityShipped</t>
+  </si>
+  <si>
+    <t>Broadcloth.dbo.ShipmentItem.QuantityShipped</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.Compliance</t>
+  </si>
+  <si>
+    <t>Broadcloth.dbo.Compliance</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.DimCompliance.ComplianceID</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.DimCompliance.DateObserved</t>
+  </si>
+  <si>
+    <t>Broadcloth .dbo.Compliance.DateObserved</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.DimCompliance.OverallRating</t>
+  </si>
+  <si>
+    <t>Broadcloth.dbo.Compliance.OverallRating</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.DimCompliance.ConditionCategory</t>
+  </si>
+  <si>
+    <t>Broadcloth.dbo.ConditionCategory.ConditionCategory</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.DimCompliance.WorkerComments</t>
+  </si>
+  <si>
+    <t>Broadcloth.dbo.WorkerCheck.WorkerComments</t>
+  </si>
+  <si>
+    <t>nvarchar(1023)</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.DimCompliance.WorkerHealth</t>
+  </si>
+  <si>
+    <t>Broadcloth.dbo.WorkerCheck.WorkerHealth</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.DimCompliance.Age</t>
+  </si>
+  <si>
+    <t>Broadcloth.dbo.WorkerCheck.Age</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.DimCompliance.ConditionComments</t>
+  </si>
+  <si>
+    <t>Broadcloth.dbo.WorkingConditions.ConditionComments</t>
+  </si>
+  <si>
+    <t>DwBroadcloth.dbo.DimCompliance.AgeDocuments</t>
+  </si>
+  <si>
+    <t>DimensionColumn</t>
+  </si>
+  <si>
+    <t>Broadcloth.dbo.WorkerCheck.AgeDocuments</t>
+  </si>
+  <si>
+    <t>nvarchar(150)</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.Customer</t>
+  </si>
+  <si>
+    <t>Broadcloth.dbo.Customer</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.Customer.CustomerID</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.Customer.BaseCurrency</t>
+  </si>
+  <si>
+    <t>Broadcloth.dbo.Customer.BaseCurrency</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.Customer.BillPostalCode</t>
+  </si>
+  <si>
+    <t>Broadcloth.dbo.CustomerOrder.BillPostalCode</t>
+  </si>
+  <si>
+    <t>nvarcar(12)</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.Customer.OrderDate</t>
+  </si>
+  <si>
+    <t>Broadcloth.dbo.CustomerOrder.OrderDate</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.Customer.BillState</t>
+  </si>
+  <si>
+    <t>Broadcloth.dbo.CustomerOrder.BillState</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.Customer.BillNation</t>
+  </si>
+  <si>
+    <t>Broadcloth.dbo.CustomerOrder.BillNation</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.Customer.PriceAdjustment</t>
+  </si>
+  <si>
+    <t>Broadcloth.dbo.CustomerOrder.PriceAdjustment</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.DimDates</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.DimDates.Date</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.DimDates.Month</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.DimDates.MonthName</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.DimDates.Quarter</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.DimDates.QuarterName</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.DimDates.Year</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.DimDates.YearName</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.DimDates.DayOfWeek</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.DimDates.DayOfMonth</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.DimDates.DayOfYear</t>
+  </si>
+  <si>
+    <t>DWBroadcloth.dbo.DimDates.Season</t>
   </si>
 </sst>
 </file>
@@ -686,18 +717,13 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Helvetica 65 Medium"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -750,8 +776,27 @@
       <name val="Helvetica 65 Medium"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -802,13 +847,25 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA6A6A6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -962,20 +1019,20 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
@@ -983,15 +1040,15 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1001,45 +1058,56 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1382,7 +1450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1396,23 +1464,23 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="10" t="s">
-        <v>141</v>
+        <v>97</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>142</v>
+        <v>98</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>143</v>
+        <v>99</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>144</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="11" t="s">
-        <v>213</v>
-      </c>
-      <c r="B2" s="48">
+        <v>124</v>
+      </c>
+      <c r="B2" s="41">
         <v>8138628846</v>
       </c>
       <c r="C2" s="11"/>
@@ -1420,9 +1488,9 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="12" t="s">
-        <v>214</v>
-      </c>
-      <c r="B3" s="49">
+        <v>125</v>
+      </c>
+      <c r="B3" s="42">
         <v>6518956609</v>
       </c>
       <c r="C3" s="12"/>
@@ -1430,23 +1498,23 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="27" t="s">
-        <v>215</v>
-      </c>
-      <c r="B4" s="50">
+        <v>126</v>
+      </c>
+      <c r="B4" s="43">
         <v>7196715291</v>
       </c>
       <c r="C4" s="27"/>
       <c r="D4" s="27"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="51" t="s">
-        <v>216</v>
-      </c>
-      <c r="B5" s="52">
+      <c r="A5" s="44" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" s="45">
         <v>7193230319</v>
       </c>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1456,10 +1524,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A3:E48"/>
+  <dimension ref="A2:E56"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1471,779 +1539,936 @@
     <col min="5" max="5" width="19.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" ht="18">
-      <c r="A3" s="1" t="s">
+    <row r="2" spans="1:5">
+      <c r="A2" s="52" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="49" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="50" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="50" t="s">
+        <v>129</v>
+      </c>
+      <c r="D4" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="50" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="51" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="51" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="51" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="50" t="s">
+        <v>132</v>
+      </c>
+      <c r="B6" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="50" t="s">
+        <v>133</v>
+      </c>
+      <c r="D6" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="50" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="50" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="50" t="s">
+        <v>135</v>
+      </c>
+      <c r="D7" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="50" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="28.5">
+      <c r="A8" s="50" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="50" t="s">
+        <v>137</v>
+      </c>
+      <c r="D8" s="50" t="s">
+        <v>94</v>
+      </c>
+      <c r="E8" s="50" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="28.5">
+      <c r="A9" s="50" t="s">
+        <v>138</v>
+      </c>
+      <c r="B9" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C9" s="50" t="s">
+        <v>139</v>
+      </c>
+      <c r="D9" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="50" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="28.5">
+      <c r="A10" s="50" t="s">
+        <v>140</v>
+      </c>
+      <c r="B10" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" s="50" t="s">
+        <v>141</v>
+      </c>
+      <c r="D10" s="50" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" s="50" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="14.45" customHeight="1">
+      <c r="A11" s="50" t="s">
+        <v>142</v>
+      </c>
+      <c r="B11" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" s="50" t="s">
+        <v>143</v>
+      </c>
+      <c r="D11" s="50" t="s">
+        <v>94</v>
+      </c>
+      <c r="E11" s="50" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="28.5">
+      <c r="A12" s="50" t="s">
+        <v>144</v>
+      </c>
+      <c r="B12" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" s="50" t="s">
+        <v>145</v>
+      </c>
+      <c r="D12" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="E12" s="50" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="28.5">
+      <c r="A13" s="50" t="s">
+        <v>147</v>
+      </c>
+      <c r="B13" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="D13" s="50" t="s">
+        <v>149</v>
+      </c>
+      <c r="E13" s="50" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="28.5">
+      <c r="A14" s="50" t="s">
+        <v>150</v>
+      </c>
+      <c r="B14" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" s="50" t="s">
+        <v>151</v>
+      </c>
+      <c r="D14" s="50" t="s">
+        <v>94</v>
+      </c>
+      <c r="E14" s="50" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="50" t="s">
+        <v>152</v>
+      </c>
+      <c r="B15" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="50" t="s">
+        <v>153</v>
+      </c>
+      <c r="D15" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="50" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="28.5">
+      <c r="A16" s="50" t="s">
+        <v>154</v>
+      </c>
+      <c r="B16" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="50" t="s">
+        <v>155</v>
+      </c>
+      <c r="D16" s="50" t="s">
+        <v>156</v>
+      </c>
+      <c r="E16" s="50" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="51" t="s">
+        <v>157</v>
+      </c>
+      <c r="B17" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="51" t="s">
+        <v>158</v>
+      </c>
+      <c r="D17" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="51" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="50" t="s">
+        <v>159</v>
+      </c>
+      <c r="B18" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="50" t="s">
+        <v>160</v>
+      </c>
+      <c r="D18" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="E18" s="50" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="50" t="s">
+        <v>161</v>
+      </c>
+      <c r="B19" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C19" s="50" t="s">
+        <v>162</v>
+      </c>
+      <c r="D19" s="50" t="s">
+        <v>102</v>
+      </c>
+      <c r="E19" s="50" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="50" t="s">
+        <v>163</v>
+      </c>
+      <c r="B20" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C20" s="50" t="s">
+        <v>164</v>
+      </c>
+      <c r="D20" s="50" t="s">
+        <v>94</v>
+      </c>
+      <c r="E20" s="50" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="50" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="36" t="s">
+      <c r="B21" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C21" s="50" t="s">
+        <v>166</v>
+      </c>
+      <c r="D21" s="50" t="s">
+        <v>167</v>
+      </c>
+      <c r="E21" s="50" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="50" t="s">
+        <v>168</v>
+      </c>
+      <c r="B22" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C22" s="50" t="s">
+        <v>169</v>
+      </c>
+      <c r="D22" s="50" t="s">
+        <v>170</v>
+      </c>
+      <c r="E22" s="50" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="50" t="s">
+        <v>171</v>
+      </c>
+      <c r="B23" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C23" s="50" t="s">
+        <v>172</v>
+      </c>
+      <c r="D23" s="50" t="s">
+        <v>102</v>
+      </c>
+      <c r="E23" s="50" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="50" t="s">
+        <v>173</v>
+      </c>
+      <c r="B24" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" s="50" t="s">
+        <v>174</v>
+      </c>
+      <c r="D24" s="50" t="s">
+        <v>149</v>
+      </c>
+      <c r="E24" s="50" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="28.5">
+      <c r="A25" s="50" t="s">
+        <v>175</v>
+      </c>
+      <c r="B25" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C25" s="50" t="s">
+        <v>176</v>
+      </c>
+      <c r="D25" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="50" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="51" t="s">
+        <v>177</v>
+      </c>
+      <c r="B26" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" s="51" t="s">
+        <v>178</v>
+      </c>
+      <c r="D26" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="51" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="50" t="s">
+        <v>179</v>
+      </c>
+      <c r="B27" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="50" t="s">
+        <v>103</v>
+      </c>
+      <c r="D27" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="E27" s="50" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="28.5">
+      <c r="A28" s="50" t="s">
+        <v>180</v>
+      </c>
+      <c r="B28" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C28" s="50" t="s">
+        <v>181</v>
+      </c>
+      <c r="D28" s="50" t="s">
+        <v>94</v>
+      </c>
+      <c r="E28" s="50" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="50" t="s">
+        <v>182</v>
+      </c>
+      <c r="B29" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C29" s="50" t="s">
+        <v>183</v>
+      </c>
+      <c r="D29" s="50" t="s">
+        <v>156</v>
+      </c>
+      <c r="E29" s="50" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="28.5">
+      <c r="A30" s="50" t="s">
+        <v>184</v>
+      </c>
+      <c r="B30" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C30" s="50" t="s">
+        <v>185</v>
+      </c>
+      <c r="D30" s="50" t="s">
+        <v>102</v>
+      </c>
+      <c r="E30" s="50" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="28.5">
+      <c r="A31" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="B31" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C31" s="50" t="s">
+        <v>187</v>
+      </c>
+      <c r="D31" s="50" t="s">
+        <v>188</v>
+      </c>
+      <c r="E31" s="50" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="28.5">
+      <c r="A32" s="50" t="s">
+        <v>189</v>
+      </c>
+      <c r="B32" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C32" s="50" t="s">
+        <v>190</v>
+      </c>
+      <c r="D32" s="50" t="s">
+        <v>188</v>
+      </c>
+      <c r="E32" s="50" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="50" t="s">
+        <v>191</v>
+      </c>
+      <c r="B33" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C33" s="50" t="s">
+        <v>192</v>
+      </c>
+      <c r="D33" s="50" t="s">
+        <v>156</v>
+      </c>
+      <c r="E33" s="50" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="14.45" customHeight="1">
+      <c r="A34" s="50" t="s">
+        <v>193</v>
+      </c>
+      <c r="B34" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C34" s="50" t="s">
+        <v>194</v>
+      </c>
+      <c r="D34" s="50" t="s">
+        <v>188</v>
+      </c>
+      <c r="E34" s="50" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="28.5">
+      <c r="A35" s="50" t="s">
+        <v>195</v>
+      </c>
+      <c r="B35" s="50" t="s">
+        <v>196</v>
+      </c>
+      <c r="C35" s="50" t="s">
+        <v>197</v>
+      </c>
+      <c r="D35" s="50" t="s">
+        <v>198</v>
+      </c>
+      <c r="E35" s="50" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="51" t="s">
+        <v>199</v>
+      </c>
+      <c r="B36" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="C36" s="51" t="s">
+        <v>200</v>
+      </c>
+      <c r="D36" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="51" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="50" t="s">
+        <v>201</v>
+      </c>
+      <c r="B37" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="50" t="s">
+        <v>103</v>
+      </c>
+      <c r="D37" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="E37" s="50" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="50" t="s">
+        <v>202</v>
+      </c>
+      <c r="B38" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C38" s="50" t="s">
+        <v>203</v>
+      </c>
+      <c r="D38" s="50" t="s">
+        <v>170</v>
+      </c>
+      <c r="E38" s="50" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="28.5">
+      <c r="A39" s="50" t="s">
+        <v>204</v>
+      </c>
+      <c r="B39" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C39" s="50" t="s">
+        <v>205</v>
+      </c>
+      <c r="D39" s="50" t="s">
+        <v>206</v>
+      </c>
+      <c r="E39" s="50" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="50" t="s">
+        <v>207</v>
+      </c>
+      <c r="B40" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C40" s="50" t="s">
+        <v>208</v>
+      </c>
+      <c r="D40" s="50" t="s">
+        <v>94</v>
+      </c>
+      <c r="E40" s="50" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="B41" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C41" s="50" t="s">
+        <v>210</v>
+      </c>
+      <c r="D41" s="50" t="s">
+        <v>170</v>
+      </c>
+      <c r="E41" s="50" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="50" t="s">
+        <v>211</v>
+      </c>
+      <c r="B42" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C42" s="50" t="s">
+        <v>212</v>
+      </c>
+      <c r="D42" s="50" t="s">
+        <v>102</v>
+      </c>
+      <c r="E42" s="50" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="28.5">
+      <c r="A43" s="50" t="s">
+        <v>213</v>
+      </c>
+      <c r="B43" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C43" s="50" t="s">
+        <v>214</v>
+      </c>
+      <c r="D43" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="E43" s="50" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="47" t="s">
+        <v>215</v>
+      </c>
+      <c r="B44" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="C44" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="D44" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="E44" s="47" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="50" t="s">
+        <v>216</v>
+      </c>
+      <c r="B45" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C45" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="D45" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="E45" s="50" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="50" t="s">
+        <v>217</v>
+      </c>
+      <c r="B46" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C46" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="D46" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="E46" s="50" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="50" t="s">
+        <v>218</v>
+      </c>
+      <c r="B47" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C47" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="D47" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="E47" s="50" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="50" t="s">
+        <v>219</v>
+      </c>
+      <c r="B48" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C48" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="D48" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="E48" s="50" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="50" t="s">
+        <v>220</v>
+      </c>
+      <c r="B49" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C49" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="D49" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="E49" s="50" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="50" t="s">
+        <v>221</v>
+      </c>
+      <c r="B50" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C50" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="D50" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="E50" s="50" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="50" t="s">
+        <v>222</v>
+      </c>
+      <c r="B51" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C51" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="D51" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="E51" s="50" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="50" t="s">
+        <v>223</v>
+      </c>
+      <c r="B52" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C52" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="D52" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="E52" s="50" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="50" t="s">
+        <v>224</v>
+      </c>
+      <c r="B53" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C53" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="D53" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="E53" s="50" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="50" t="s">
+        <v>225</v>
+      </c>
+      <c r="B54" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C54" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="D54" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="E54" s="50" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="50" t="s">
+        <v>226</v>
+      </c>
+      <c r="B55" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C55" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="D55" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="E55" s="50" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="36" t="s">
+      <c r="B56" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="C56" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="36" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="37" t="s">
-        <v>98</v>
-      </c>
-      <c r="B5" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="37" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="38" t="s">
-        <v>99</v>
-      </c>
-      <c r="B6" s="38" t="s">
+      <c r="D56" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="38" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="39" t="s">
-        <v>160</v>
-      </c>
-      <c r="B7" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="39" t="s">
-        <v>118</v>
-      </c>
-      <c r="D7" s="39" t="s">
-        <v>108</v>
-      </c>
-      <c r="E7" s="39" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="39" t="s">
-        <v>105</v>
-      </c>
-      <c r="B8" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="39" t="s">
-        <v>119</v>
-      </c>
-      <c r="D8" s="39" t="s">
-        <v>109</v>
-      </c>
-      <c r="E8" s="39" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="39" t="s">
-        <v>100</v>
-      </c>
-      <c r="B9" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="39" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="39" t="s">
-        <v>106</v>
-      </c>
-      <c r="E9" s="39" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="39" t="s">
-        <v>104</v>
-      </c>
-      <c r="B10" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="39" t="s">
-        <v>103</v>
-      </c>
-      <c r="D10" s="39" t="s">
-        <v>107</v>
-      </c>
-      <c r="E10" s="39" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="14.45" customHeight="1">
-      <c r="A11" s="39" t="s">
-        <v>102</v>
-      </c>
-      <c r="B11" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="39" t="s">
+      <c r="E56" s="49" t="s">
         <v>9</v>
-      </c>
-      <c r="D11" s="39" t="s">
-        <v>198</v>
-      </c>
-      <c r="E11" s="39" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="38" t="s">
-        <v>132</v>
-      </c>
-      <c r="B12" s="38" t="s">
-        <v>131</v>
-      </c>
-      <c r="C12" s="38" t="s">
-        <v>110</v>
-      </c>
-      <c r="D12" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="38" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="39" t="s">
-        <v>154</v>
-      </c>
-      <c r="B13" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="39" t="s">
-        <v>158</v>
-      </c>
-      <c r="D13" s="39" t="s">
-        <v>159</v>
-      </c>
-      <c r="E13" s="39" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="39" t="s">
-        <v>155</v>
-      </c>
-      <c r="B14" s="39" t="s">
-        <v>157</v>
-      </c>
-      <c r="C14" s="39" t="s">
-        <v>115</v>
-      </c>
-      <c r="D14" s="39" t="s">
-        <v>107</v>
-      </c>
-      <c r="E14" s="39" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="39" t="s">
-        <v>156</v>
-      </c>
-      <c r="B15" s="39" t="s">
-        <v>145</v>
-      </c>
-      <c r="C15" s="39" t="s">
-        <v>116</v>
-      </c>
-      <c r="D15" s="39" t="s">
-        <v>147</v>
-      </c>
-      <c r="E15" s="39" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="38" t="s">
-        <v>101</v>
-      </c>
-      <c r="B16" s="38" t="s">
-        <v>131</v>
-      </c>
-      <c r="C16" s="38" t="s">
-        <v>111</v>
-      </c>
-      <c r="D16" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="38" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="39" t="s">
-        <v>186</v>
-      </c>
-      <c r="B17" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="39" t="s">
-        <v>158</v>
-      </c>
-      <c r="D17" s="39" t="s">
-        <v>159</v>
-      </c>
-      <c r="E17" s="39" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="39" t="s">
-        <v>187</v>
-      </c>
-      <c r="B18" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="39" t="s">
-        <v>117</v>
-      </c>
-      <c r="D18" s="39" t="s">
-        <v>106</v>
-      </c>
-      <c r="E18" s="39" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="39" t="s">
-        <v>188</v>
-      </c>
-      <c r="B19" s="39" t="s">
-        <v>145</v>
-      </c>
-      <c r="C19" s="39" t="s">
-        <v>120</v>
-      </c>
-      <c r="D19" s="39" t="s">
-        <v>149</v>
-      </c>
-      <c r="E19" s="39" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="39" t="s">
-        <v>189</v>
-      </c>
-      <c r="B20" s="39" t="s">
-        <v>145</v>
-      </c>
-      <c r="C20" s="39" t="s">
-        <v>121</v>
-      </c>
-      <c r="D20" s="39" t="s">
-        <v>150</v>
-      </c>
-      <c r="E20" s="39" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="39" t="s">
-        <v>190</v>
-      </c>
-      <c r="B21" s="39" t="s">
-        <v>145</v>
-      </c>
-      <c r="C21" s="39" t="s">
-        <v>122</v>
-      </c>
-      <c r="D21" s="39" t="s">
-        <v>107</v>
-      </c>
-      <c r="E21" s="39" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="39" t="s">
-        <v>191</v>
-      </c>
-      <c r="B22" s="39" t="s">
-        <v>145</v>
-      </c>
-      <c r="C22" s="39" t="s">
-        <v>123</v>
-      </c>
-      <c r="D22" s="39" t="s">
-        <v>151</v>
-      </c>
-      <c r="E22" s="39" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="39" t="s">
-        <v>192</v>
-      </c>
-      <c r="B23" s="39" t="s">
-        <v>145</v>
-      </c>
-      <c r="C23" s="39" t="s">
-        <v>124</v>
-      </c>
-      <c r="D23" s="39" t="s">
-        <v>109</v>
-      </c>
-      <c r="E23" s="39" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="38" t="s">
-        <v>133</v>
-      </c>
-      <c r="B24" s="38" t="s">
-        <v>131</v>
-      </c>
-      <c r="C24" s="38" t="s">
-        <v>112</v>
-      </c>
-      <c r="D24" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" s="38" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="39" t="s">
-        <v>193</v>
-      </c>
-      <c r="B25" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="39" t="s">
-        <v>158</v>
-      </c>
-      <c r="D25" s="39" t="s">
-        <v>159</v>
-      </c>
-      <c r="E25" s="39" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="39" t="s">
-        <v>194</v>
-      </c>
-      <c r="B26" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="39" t="s">
-        <v>125</v>
-      </c>
-      <c r="D26" s="39" t="s">
-        <v>107</v>
-      </c>
-      <c r="E26" s="39" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="39" t="s">
-        <v>195</v>
-      </c>
-      <c r="B27" s="39" t="s">
-        <v>145</v>
-      </c>
-      <c r="C27" s="39" t="s">
-        <v>126</v>
-      </c>
-      <c r="D27" s="39" t="s">
-        <v>147</v>
-      </c>
-      <c r="E27" s="39" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="38" t="s">
-        <v>181</v>
-      </c>
-      <c r="B28" s="38" t="s">
-        <v>131</v>
-      </c>
-      <c r="C28" s="38" t="s">
-        <v>113</v>
-      </c>
-      <c r="D28" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="E28" s="38" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="39" t="s">
-        <v>182</v>
-      </c>
-      <c r="B29" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="C29" s="39" t="s">
-        <v>201</v>
-      </c>
-      <c r="D29" s="39" t="s">
-        <v>159</v>
-      </c>
-      <c r="E29" s="39" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="39" t="s">
-        <v>183</v>
-      </c>
-      <c r="B30" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="C30" s="39" t="s">
-        <v>200</v>
-      </c>
-      <c r="D30" s="39" t="s">
-        <v>159</v>
-      </c>
-      <c r="E30" s="39" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="39" t="s">
-        <v>184</v>
-      </c>
-      <c r="B31" s="39" t="s">
-        <v>145</v>
-      </c>
-      <c r="C31" s="39" t="s">
-        <v>127</v>
-      </c>
-      <c r="D31" s="39" t="s">
-        <v>152</v>
-      </c>
-      <c r="E31" s="39" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="38" t="s">
-        <v>134</v>
-      </c>
-      <c r="B32" s="38" t="s">
-        <v>131</v>
-      </c>
-      <c r="C32" s="38" t="s">
-        <v>114</v>
-      </c>
-      <c r="D32" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" s="38" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="B33" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="C33" s="39" t="s">
-        <v>158</v>
-      </c>
-      <c r="D33" s="39" t="s">
-        <v>159</v>
-      </c>
-      <c r="E33" s="39" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="14.45" customHeight="1">
-      <c r="A34" s="39" t="s">
-        <v>138</v>
-      </c>
-      <c r="B34" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="C34" s="39" t="s">
-        <v>128</v>
-      </c>
-      <c r="D34" s="39" t="s">
-        <v>146</v>
-      </c>
-      <c r="E34" s="39" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="39" t="s">
-        <v>136</v>
-      </c>
-      <c r="B35" s="39" t="s">
-        <v>145</v>
-      </c>
-      <c r="C35" s="39" t="s">
-        <v>135</v>
-      </c>
-      <c r="D35" s="39" t="s">
-        <v>147</v>
-      </c>
-      <c r="E35" s="39" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="41" t="s">
-        <v>136</v>
-      </c>
-      <c r="B36" s="41" t="s">
-        <v>145</v>
-      </c>
-      <c r="C36" s="41" t="s">
-        <v>129</v>
-      </c>
-      <c r="D36" s="41" t="s">
-        <v>108</v>
-      </c>
-      <c r="E36" s="41" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="41" t="s">
-        <v>137</v>
-      </c>
-      <c r="B37" s="41" t="s">
-        <v>145</v>
-      </c>
-      <c r="C37" s="41" t="s">
-        <v>130</v>
-      </c>
-      <c r="D37" s="41" t="s">
-        <v>148</v>
-      </c>
-      <c r="E37" s="41" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="42" t="s">
-        <v>203</v>
-      </c>
-      <c r="B38" s="38" t="s">
-        <v>131</v>
-      </c>
-      <c r="C38" s="43" t="s">
-        <v>159</v>
-      </c>
-      <c r="D38" s="42" t="s">
-        <v>159</v>
-      </c>
-      <c r="E38" s="42" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="41" t="s">
-        <v>202</v>
-      </c>
-      <c r="B39" s="41" t="s">
-        <v>145</v>
-      </c>
-      <c r="C39" s="41" t="s">
-        <v>159</v>
-      </c>
-      <c r="D39" s="41" t="s">
-        <v>159</v>
-      </c>
-      <c r="E39" s="41" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="41" t="s">
-        <v>212</v>
-      </c>
-      <c r="B40" s="41" t="s">
-        <v>145</v>
-      </c>
-      <c r="C40" s="41" t="s">
-        <v>159</v>
-      </c>
-      <c r="D40" s="41" t="s">
-        <v>159</v>
-      </c>
-      <c r="E40" s="41" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="39" t="s">
-        <v>204</v>
-      </c>
-      <c r="B41" s="41" t="s">
-        <v>145</v>
-      </c>
-      <c r="C41" s="41" t="s">
-        <v>159</v>
-      </c>
-      <c r="D41" s="41" t="s">
-        <v>159</v>
-      </c>
-      <c r="E41" s="41" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="39" t="s">
-        <v>207</v>
-      </c>
-      <c r="B42" s="41" t="s">
-        <v>145</v>
-      </c>
-      <c r="C42" s="41" t="s">
-        <v>159</v>
-      </c>
-      <c r="D42" s="41" t="s">
-        <v>159</v>
-      </c>
-      <c r="E42" s="41" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="39" t="s">
-        <v>205</v>
-      </c>
-      <c r="B43" s="41" t="s">
-        <v>145</v>
-      </c>
-      <c r="C43" s="39" t="s">
-        <v>159</v>
-      </c>
-      <c r="D43" s="39" t="s">
-        <v>159</v>
-      </c>
-      <c r="E43" s="41" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="39" t="s">
-        <v>206</v>
-      </c>
-      <c r="B44" s="41" t="s">
-        <v>145</v>
-      </c>
-      <c r="C44" s="39" t="s">
-        <v>159</v>
-      </c>
-      <c r="D44" s="39" t="s">
-        <v>159</v>
-      </c>
-      <c r="E44" s="41" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="39" t="s">
-        <v>208</v>
-      </c>
-      <c r="B45" s="41" t="s">
-        <v>145</v>
-      </c>
-      <c r="C45" s="39" t="s">
-        <v>159</v>
-      </c>
-      <c r="D45" s="39" t="s">
-        <v>159</v>
-      </c>
-      <c r="E45" s="41" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="39" t="s">
-        <v>209</v>
-      </c>
-      <c r="B46" s="41" t="s">
-        <v>145</v>
-      </c>
-      <c r="C46" s="39" t="s">
-        <v>159</v>
-      </c>
-      <c r="D46" s="39" t="s">
-        <v>159</v>
-      </c>
-      <c r="E46" s="41" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="39" t="s">
-        <v>210</v>
-      </c>
-      <c r="B47" s="41" t="s">
-        <v>145</v>
-      </c>
-      <c r="C47" s="39" t="s">
-        <v>159</v>
-      </c>
-      <c r="D47" s="39" t="s">
-        <v>159</v>
-      </c>
-      <c r="E47" s="41" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B48" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="C48" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="D48" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="E48" s="36" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2263,74 +2488,74 @@
   <sheetData>
     <row r="2" spans="1:2">
       <c r="A2" s="10" t="s">
-        <v>140</v>
+        <v>96</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>141</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="11" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="12" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="11" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="12" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="11" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="12" t="s">
         <v>92</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="11" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>93</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2354,51 +2579,51 @@
   <sheetData>
     <row r="2" spans="1:12">
       <c r="A2" s="15" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>171</v>
+        <v>111</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>166</v>
+        <v>106</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>167</v>
+        <v>107</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>168</v>
+        <v>108</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>169</v>
+        <v>109</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>170</v>
+        <v>110</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>166</v>
+        <v>106</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>167</v>
+        <v>107</v>
       </c>
       <c r="J2" s="15" t="s">
-        <v>168</v>
+        <v>108</v>
       </c>
       <c r="K2" s="15" t="s">
-        <v>169</v>
+        <v>109</v>
       </c>
       <c r="L2" s="15" t="s">
-        <v>170</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B3" s="11">
         <v>28</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>172</v>
+        <v>112</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
@@ -2412,7 +2637,7 @@
     </row>
     <row r="4" spans="1:12" ht="14.65" thickBot="1">
       <c r="A4" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B4" s="11">
         <v>18</v>
@@ -2421,7 +2646,7 @@
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
       <c r="F4" s="18" t="s">
-        <v>173</v>
+        <v>113</v>
       </c>
       <c r="G4" s="17"/>
       <c r="H4" s="17"/>
@@ -2432,7 +2657,7 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="22" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B5" s="23">
         <v>3</v>
@@ -2443,7 +2668,7 @@
       <c r="F5" s="23"/>
       <c r="G5" s="23"/>
       <c r="H5" s="24" t="s">
-        <v>174</v>
+        <v>114</v>
       </c>
       <c r="I5" s="23"/>
       <c r="J5" s="23"/>
@@ -2452,7 +2677,7 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="26" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B6" s="27">
         <v>6</v>
@@ -2463,7 +2688,7 @@
       <c r="F6" s="27"/>
       <c r="G6" s="27"/>
       <c r="H6" s="28" t="s">
-        <v>175</v>
+        <v>115</v>
       </c>
       <c r="I6" s="29"/>
       <c r="J6" s="27"/>
@@ -2472,7 +2697,7 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="26" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B7" s="27">
         <v>6</v>
@@ -2483,7 +2708,7 @@
       <c r="F7" s="27"/>
       <c r="G7" s="27"/>
       <c r="H7" s="28" t="s">
-        <v>176</v>
+        <v>116</v>
       </c>
       <c r="I7" s="27"/>
       <c r="J7" s="27"/>
@@ -2492,7 +2717,7 @@
     </row>
     <row r="8" spans="1:12" ht="14.65" thickBot="1">
       <c r="A8" s="31" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B8" s="32">
         <v>6</v>
@@ -2503,7 +2728,7 @@
       <c r="F8" s="32"/>
       <c r="G8" s="32"/>
       <c r="H8" s="33" t="s">
-        <v>176</v>
+        <v>116</v>
       </c>
       <c r="I8" s="32"/>
       <c r="J8" s="32"/>
@@ -2512,7 +2737,7 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B9" s="11">
         <v>21</v>
@@ -2523,10 +2748,10 @@
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
       <c r="H9" s="19" t="s">
-        <v>178</v>
+        <v>118</v>
       </c>
       <c r="I9" s="18" t="s">
-        <v>177</v>
+        <v>117</v>
       </c>
       <c r="J9" s="17"/>
       <c r="K9" s="17"/>
@@ -2534,7 +2759,7 @@
     </row>
     <row r="10" spans="1:12" ht="28.5">
       <c r="A10" s="16" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B10" s="13">
         <v>9</v>
@@ -2548,7 +2773,7 @@
       <c r="I10" s="13"/>
       <c r="J10" s="13"/>
       <c r="K10" s="21" t="s">
-        <v>179</v>
+        <v>119</v>
       </c>
       <c r="L10" s="20"/>
     </row>
@@ -2586,30 +2811,30 @@
   <sheetData>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -2618,7 +2843,7 @@
     <row r="4" spans="1:5">
       <c r="A4" s="3"/>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -2627,7 +2852,7 @@
     <row r="5" spans="1:5">
       <c r="A5" s="3"/>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -2636,7 +2861,7 @@
     <row r="6" spans="1:5">
       <c r="A6" s="3"/>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -2645,10 +2870,10 @@
     <row r="7" spans="1:5">
       <c r="A7" s="3"/>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D7">
         <v>3</v>
@@ -2657,7 +2882,7 @@
     <row r="8" spans="1:5">
       <c r="A8" s="3"/>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D8">
         <v>3</v>
@@ -2666,10 +2891,10 @@
     <row r="9" spans="1:5">
       <c r="A9" s="3"/>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D9">
         <v>3</v>
@@ -2678,7 +2903,7 @@
     <row r="10" spans="1:5">
       <c r="A10" s="3"/>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D10">
         <v>3</v>
@@ -2687,7 +2912,7 @@
     <row r="11" spans="1:5">
       <c r="A11" s="3"/>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D11">
         <v>3</v>
@@ -2696,10 +2921,10 @@
     <row r="12" spans="1:5">
       <c r="A12" s="3"/>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -2717,13 +2942,13 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -2732,10 +2957,10 @@
     <row r="15" spans="1:5">
       <c r="A15" s="3"/>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -2744,10 +2969,10 @@
     <row r="16" spans="1:5">
       <c r="A16" s="3"/>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -2756,10 +2981,10 @@
     <row r="17" spans="1:5">
       <c r="A17" s="3"/>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -2768,10 +2993,10 @@
     <row r="18" spans="1:5">
       <c r="A18" s="3"/>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C18" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -2780,7 +3005,7 @@
     <row r="19" spans="1:5">
       <c r="A19" s="3"/>
       <c r="C19" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -2789,10 +3014,10 @@
     <row r="20" spans="1:5">
       <c r="A20" s="3"/>
       <c r="B20" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -2801,10 +3026,10 @@
     <row r="21" spans="1:5">
       <c r="A21" s="3"/>
       <c r="B21" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C21" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D21">
         <v>3</v>
@@ -2813,10 +3038,10 @@
     <row r="22" spans="1:5">
       <c r="A22" s="3"/>
       <c r="B22" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C22" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -2825,10 +3050,10 @@
     <row r="23" spans="1:5">
       <c r="A23" s="3"/>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C23" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -2837,10 +3062,10 @@
     <row r="24" spans="1:5">
       <c r="A24" s="3"/>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C24" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D24">
         <v>3</v>
@@ -2849,7 +3074,7 @@
     <row r="25" spans="1:5">
       <c r="A25" s="3"/>
       <c r="C25" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D25">
         <v>3</v>
@@ -2867,13 +3092,13 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C27" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D27">
         <v>2</v>
@@ -2882,7 +3107,7 @@
     <row r="28" spans="1:5">
       <c r="A28" s="3"/>
       <c r="C28" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -2900,13 +3125,13 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C30" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D30">
         <v>3</v>
@@ -2915,7 +3140,7 @@
     <row r="31" spans="1:5">
       <c r="A31" s="3"/>
       <c r="C31" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D31">
         <v>3</v>
@@ -2933,13 +3158,13 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C33" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D33">
         <v>3</v>
@@ -2948,7 +3173,7 @@
     <row r="34" spans="1:5">
       <c r="A34" s="3"/>
       <c r="C34" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D34">
         <v>3</v>
@@ -2966,13 +3191,13 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B36" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C36" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D36">
         <v>3</v>
@@ -2981,7 +3206,7 @@
     <row r="37" spans="1:5">
       <c r="A37" s="3"/>
       <c r="C37" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D37">
         <v>3</v>
@@ -2999,13 +3224,13 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B39" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C39" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D39">
         <v>3</v>
@@ -3014,7 +3239,7 @@
     <row r="40" spans="1:5">
       <c r="A40" s="3"/>
       <c r="C40" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D40">
         <v>3</v>
@@ -3023,7 +3248,7 @@
     <row r="41" spans="1:5">
       <c r="A41" s="3"/>
       <c r="C41" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D41">
         <v>3</v>
@@ -3032,7 +3257,7 @@
     <row r="42" spans="1:5">
       <c r="A42" s="3"/>
       <c r="C42" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D42">
         <v>3</v>
@@ -3041,10 +3266,10 @@
     <row r="43" spans="1:5">
       <c r="A43" s="3"/>
       <c r="B43" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C43" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D43">
         <v>3</v>
@@ -3053,7 +3278,7 @@
     <row r="44" spans="1:5">
       <c r="A44" s="3"/>
       <c r="C44" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D44">
         <v>3</v>
@@ -3062,7 +3287,7 @@
     <row r="45" spans="1:5">
       <c r="A45" s="3"/>
       <c r="C45" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D45">
         <v>3</v>
@@ -3079,23 +3304,23 @@
       <c r="E46" s="7"/>
     </row>
     <row r="47" spans="1:5" ht="12.6" customHeight="1">
-      <c r="A47" s="53" t="s">
-        <v>38</v>
+      <c r="A47" s="46" t="s">
+        <v>34</v>
       </c>
       <c r="B47" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C47" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D47">
         <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:5">
-      <c r="A48" s="53"/>
+      <c r="A48" s="46"/>
       <c r="C48" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D48">
         <v>3</v>
@@ -3104,7 +3329,7 @@
     <row r="49" spans="1:5">
       <c r="A49" s="4"/>
       <c r="C49" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D49">
         <v>3</v>
@@ -3127,7 +3352,7 @@
       <c r="A52" s="5"/>
       <c r="B52" s="9"/>
       <c r="C52" s="9" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D52" s="5">
         <f>SUM(D50,D46,D38,D35,D32,D29,D26,D13) * 1.1</f>
@@ -3161,107 +3386,107 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="17.649999999999999">
-      <c r="A2" s="44" t="s">
-        <v>180</v>
-      </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
+      <c r="A2" s="37" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" s="37"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="45" t="s">
-        <v>211</v>
-      </c>
-      <c r="C3" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="45" t="s">
+      <c r="B3" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="45" t="s">
-        <v>197</v>
+      <c r="E3" s="38" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="46"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="46"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
+      <c r="A5" s="39"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="47"/>
-      <c r="B6" s="47"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
+      <c r="A6" s="40"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="46"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
+      <c r="A7" s="39"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="47"/>
-      <c r="B8" s="47"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
+      <c r="A8" s="40"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="47"/>
-      <c r="B9" s="47"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
+      <c r="A9" s="40"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="47"/>
-      <c r="B10" s="47"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
+      <c r="A10" s="40"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="47"/>
-      <c r="B11" s="47"/>
-      <c r="C11" s="47"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
+      <c r="A11" s="40"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="46"/>
-      <c r="B12" s="46"/>
-      <c r="C12" s="46"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
+      <c r="A12" s="39"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="47"/>
-      <c r="B13" s="47"/>
-      <c r="C13" s="47"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
+      <c r="A13" s="40"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="47"/>
-      <c r="B14" s="47"/>
-      <c r="C14" s="47"/>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
+      <c r="A14" s="40"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3285,7 +3510,7 @@
   <sheetData>
     <row r="2" spans="1:2" ht="18">
       <c r="A2" s="1" t="s">
-        <v>185</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -3293,7 +3518,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>